<commit_message>
new field in xml and excels
</commit_message>
<xml_diff>
--- a/helpers/templates/delivery/ordn.xlsx
+++ b/helpers/templates/delivery/ordn.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="177">
   <si>
     <t>DocNum</t>
   </si>
@@ -323,6 +323,15 @@
   </si>
   <si>
     <t>U_ID_WMS</t>
+  </si>
+  <si>
+    <t>U_N_Tarja</t>
+  </si>
+  <si>
+    <t>U_Regimen</t>
+  </si>
+  <si>
+    <t>U_Proveedor</t>
   </si>
   <si>
     <t>U_Fecha_Pago</t>
@@ -946,7 +955,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:CZ2"/>
+  <dimension ref="A1:DC2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -1054,11 +1063,14 @@
     <col min="100" max="100" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="101" max="101" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="102" max="102" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="103" max="103" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="104" max="104" style="6" width="12.43357142857143" customWidth="1" bestFit="1" hidden="1"/>
+    <col min="103" max="103" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="104" max="104" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="105" max="105" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="106" max="106" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="107" max="107" style="6" width="13.576428571428572" customWidth="1" bestFit="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1371,8 +1383,17 @@
       <c r="CZ1" s="3" t="s">
         <v>103</v>
       </c>
+      <c r="DA1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC1" s="3" t="s">
+        <v>106</v>
+      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1401,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>3</v>
@@ -1404,7 +1425,7 @@
         <v>9</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>11</v>
@@ -1413,40 +1434,40 @@
         <v>12</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="P2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="S2" s="4" t="s">
         <v>18</v>
       </c>
       <c r="T2" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>21</v>
       </c>
       <c r="W2" s="4" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>25</v>
@@ -1458,10 +1479,10 @@
         <v>27</v>
       </c>
       <c r="AC2" s="4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="AD2" s="4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="AE2" s="4" t="s">
         <v>30</v>
@@ -1470,16 +1491,16 @@
         <v>31</v>
       </c>
       <c r="AG2" s="4" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="AH2" s="4" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="AJ2" s="4" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="AK2" s="4" t="s">
         <v>36</v>
@@ -1491,88 +1512,88 @@
         <v>38</v>
       </c>
       <c r="AN2" s="4" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="AO2" s="4" t="s">
         <v>40</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="AQ2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="AR2" s="4" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="AT2" s="4" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="AU2" s="4" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="AV2" s="4" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="AW2" s="4" t="s">
         <v>48</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="AY2" s="4" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="BA2" s="4" t="s">
         <v>52</v>
       </c>
       <c r="BB2" s="4" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="BC2" s="4" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="BD2" s="4" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="BE2" s="4" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="BF2" s="4" t="s">
         <v>57</v>
       </c>
       <c r="BG2" s="4" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="BH2" s="4" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="BI2" s="4" t="s">
         <v>60</v>
       </c>
       <c r="BJ2" s="4" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="BK2" s="4" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="BL2" s="4" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="BM2" s="4" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="BN2" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="BO2" s="4" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="BP2" s="4" t="s">
         <v>67</v>
@@ -1581,109 +1602,118 @@
         <v>68</v>
       </c>
       <c r="BR2" s="4" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="BS2" s="4" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="BT2" s="4" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="BV2" s="4" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="BW2" s="4" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="BX2" s="4" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="BY2" s="4" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="CA2" s="4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="CC2" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="CG2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="CH2" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="CI2" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="CJ2" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="CK2" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CM2" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="CD2" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="CE2" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="CF2" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="CG2" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="CH2" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="CI2" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="CJ2" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="CK2" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="CL2" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="CM2" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="CN2" s="4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="CO2" s="4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="CP2" s="4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="CQ2" s="4" t="s">
         <v>94</v>
       </c>
       <c r="CR2" s="4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="CS2" s="4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="CT2" s="4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="CU2" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="CV2" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="CW2" s="4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="CX2" s="4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="CY2" s="2" t="s">
         <v>102</v>
       </c>
       <c r="CZ2" s="3" t="s">
         <v>103</v>
+      </c>
+      <c r="DA2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="DB2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="DC2" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>